<commit_message>
update labels and add new variables
</commit_message>
<xml_diff>
--- a/Diagnoskoder/labelDictionary.xlsx
+++ b/Diagnoskoder/labelDictionary.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="206">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="211">
   <si>
     <t>K_Malder</t>
   </si>
@@ -642,6 +642,21 @@
   </si>
   <si>
     <t>sectio_robson</t>
+  </si>
+  <si>
+    <t>langd_bmi</t>
+  </si>
+  <si>
+    <t>1= normallång + normalviktig</t>
+  </si>
+  <si>
+    <t>2= Kort + normalviktig</t>
+  </si>
+  <si>
+    <t>3=Normallång +övervikt</t>
+  </si>
+  <si>
+    <t>4= Kort+Övervikt</t>
   </si>
 </sst>
 </file>
@@ -959,10 +974,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C291"/>
+  <dimension ref="A1:C295"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A269" workbookViewId="0">
-      <selection activeCell="E292" sqref="E292"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1326,95 +1341,95 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>34</v>
+        <v>206</v>
       </c>
       <c r="B33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C33" t="s">
-        <v>35</v>
+        <v>207</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>34</v>
+        <v>206</v>
       </c>
       <c r="B34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C34" t="s">
-        <v>36</v>
+        <v>208</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>34</v>
+        <v>206</v>
       </c>
       <c r="B35">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C35" t="s">
-        <v>37</v>
+        <v>209</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>206</v>
       </c>
       <c r="B36">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C36" t="s">
-        <v>38</v>
+        <v>210</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B37">
         <v>0</v>
       </c>
       <c r="C37" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B38">
         <v>1</v>
       </c>
       <c r="C38" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B39">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C39" t="s">
-        <v>65</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B40">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C40" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B41">
         <v>0</v>
@@ -1425,7 +1440,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B42">
         <v>1</v>
@@ -1436,7 +1451,7 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B43">
         <v>0</v>
@@ -1447,7 +1462,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B44">
         <v>1</v>
@@ -1458,7 +1473,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -1469,7 +1484,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B46">
         <v>1</v>
@@ -1480,68 +1495,68 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="B47">
         <v>0</v>
       </c>
       <c r="C47" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>73</v>
+        <v>42</v>
       </c>
       <c r="B48">
         <v>1</v>
       </c>
       <c r="C48" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B49">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C49" t="s">
-        <v>19</v>
+        <v>65</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B50">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C50" t="s">
-        <v>20</v>
+        <v>66</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="B51">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C51" t="s">
-        <v>21</v>
+        <v>75</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>44</v>
+        <v>73</v>
       </c>
       <c r="B52">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C52" t="s">
-        <v>22</v>
+        <v>74</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
@@ -1549,54 +1564,54 @@
         <v>44</v>
       </c>
       <c r="B53">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C53" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B54">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C54" t="s">
-        <v>46</v>
+        <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B55">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C55" t="s">
-        <v>47</v>
+        <v>21</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B56">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C56" t="s">
-        <v>48</v>
+        <v>22</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B57">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C57" t="s">
-        <v>49</v>
+        <v>23</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -1604,10 +1619,10 @@
         <v>45</v>
       </c>
       <c r="B58">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C58" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
@@ -1615,136 +1630,136 @@
         <v>45</v>
       </c>
       <c r="B59">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C59" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="B60">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="C60" t="s">
-        <v>65</v>
+        <v>48</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>76</v>
+        <v>45</v>
       </c>
       <c r="B61">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C61" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="B62">
-        <v>0</v>
+        <v>5</v>
       </c>
       <c r="C62" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>77</v>
+        <v>45</v>
       </c>
       <c r="B63">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="C63" t="s">
-        <v>79</v>
+        <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="B64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C64" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>52</v>
+        <v>76</v>
       </c>
       <c r="B65">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C65" t="s">
-        <v>54</v>
+        <v>78</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>52</v>
+        <v>77</v>
       </c>
       <c r="B66">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C66" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>56</v>
+        <v>77</v>
       </c>
       <c r="B67">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C67" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B68">
         <v>1</v>
       </c>
       <c r="C68" t="s">
-        <v>66</v>
+        <v>53</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B69">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="C69" t="s">
-        <v>65</v>
+        <v>54</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="B70">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C70" t="s">
-        <v>66</v>
+        <v>55</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -1755,7 +1770,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -1766,7 +1781,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B73">
         <v>0</v>
@@ -1777,7 +1792,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -1788,123 +1803,123 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B75">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C75" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B76">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C76" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B77">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="C77" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="B78">
         <v>1</v>
       </c>
       <c r="C78" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B79">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C79" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B80">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C80" t="s">
-        <v>69</v>
+        <v>62</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="B81">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C81" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B82">
         <v>1</v>
       </c>
       <c r="C82" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B83">
         <v>2</v>
       </c>
       <c r="C83" t="s">
-        <v>90</v>
+        <v>68</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B84">
-        <v>22</v>
+        <v>3</v>
       </c>
       <c r="C84" t="s">
-        <v>105</v>
+        <v>69</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>64</v>
       </c>
       <c r="B85">
-        <v>23</v>
+        <v>4</v>
       </c>
       <c r="C85" t="s">
-        <v>106</v>
+        <v>70</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
@@ -1912,10 +1927,10 @@
         <v>83</v>
       </c>
       <c r="B86">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C86" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
@@ -1923,10 +1938,10 @@
         <v>83</v>
       </c>
       <c r="B87">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C87" t="s">
-        <v>86</v>
+        <v>90</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
@@ -1934,10 +1949,10 @@
         <v>83</v>
       </c>
       <c r="B88">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="C88" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
@@ -1945,10 +1960,10 @@
         <v>83</v>
       </c>
       <c r="B89">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="C89" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
@@ -1956,10 +1971,10 @@
         <v>83</v>
       </c>
       <c r="B90">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C90" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
@@ -1967,10 +1982,10 @@
         <v>83</v>
       </c>
       <c r="B91">
-        <v>51</v>
+        <v>4</v>
       </c>
       <c r="C91" t="s">
-        <v>100</v>
+        <v>86</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
@@ -1978,10 +1993,10 @@
         <v>83</v>
       </c>
       <c r="B92">
-        <v>52</v>
+        <v>42</v>
       </c>
       <c r="C92" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
@@ -1989,10 +2004,10 @@
         <v>83</v>
       </c>
       <c r="B93">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C93" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
@@ -2000,10 +2015,10 @@
         <v>83</v>
       </c>
       <c r="B94">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C94" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
@@ -2011,10 +2026,10 @@
         <v>83</v>
       </c>
       <c r="B95">
-        <v>7</v>
+        <v>51</v>
       </c>
       <c r="C95" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
@@ -2022,10 +2037,10 @@
         <v>83</v>
       </c>
       <c r="B96">
-        <v>8</v>
+        <v>52</v>
       </c>
       <c r="C96" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
@@ -2033,10 +2048,10 @@
         <v>83</v>
       </c>
       <c r="B97">
-        <v>81</v>
+        <v>53</v>
       </c>
       <c r="C97" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
@@ -2044,10 +2059,10 @@
         <v>83</v>
       </c>
       <c r="B98">
-        <v>82</v>
+        <v>6</v>
       </c>
       <c r="C98" t="s">
-        <v>98</v>
+        <v>88</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
@@ -2055,10 +2070,10 @@
         <v>83</v>
       </c>
       <c r="B99">
-        <v>83</v>
+        <v>7</v>
       </c>
       <c r="C99" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
@@ -2066,10 +2081,10 @@
         <v>83</v>
       </c>
       <c r="B100">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C100" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
@@ -2077,10 +2092,10 @@
         <v>83</v>
       </c>
       <c r="B101">
-        <v>10</v>
+        <v>81</v>
       </c>
       <c r="C101" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
@@ -2088,10 +2103,10 @@
         <v>83</v>
       </c>
       <c r="B102">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C102" t="s">
-        <v>94</v>
+        <v>98</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
@@ -2099,10 +2114,10 @@
         <v>83</v>
       </c>
       <c r="B103">
-        <v>102</v>
+        <v>83</v>
       </c>
       <c r="C103" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
@@ -2110,54 +2125,54 @@
         <v>83</v>
       </c>
       <c r="B104">
-        <v>103</v>
+        <v>9</v>
       </c>
       <c r="C104" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="B105">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="C105" t="s">
-        <v>108</v>
+        <v>93</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="B106">
-        <v>2</v>
+        <v>101</v>
       </c>
       <c r="C106" t="s">
-        <v>109</v>
+        <v>94</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="B107">
-        <v>3</v>
+        <v>102</v>
       </c>
       <c r="C107" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>107</v>
+        <v>83</v>
       </c>
       <c r="B108">
-        <v>4</v>
+        <v>103</v>
       </c>
       <c r="C108" t="s">
-        <v>111</v>
+        <v>96</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
@@ -2165,10 +2180,10 @@
         <v>107</v>
       </c>
       <c r="B109">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="C109" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
@@ -2176,10 +2191,10 @@
         <v>107</v>
       </c>
       <c r="B110">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C110" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
@@ -2187,10 +2202,10 @@
         <v>107</v>
       </c>
       <c r="B111">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="C111" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -2198,10 +2213,10 @@
         <v>107</v>
       </c>
       <c r="B112">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C112" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
@@ -2209,10 +2224,10 @@
         <v>107</v>
       </c>
       <c r="B113">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="C113" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
@@ -2220,10 +2235,10 @@
         <v>107</v>
       </c>
       <c r="B114">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="C114" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
@@ -2231,59 +2246,59 @@
         <v>107</v>
       </c>
       <c r="B115">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C115" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
       <c r="B116">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="C116" t="s">
-        <v>65</v>
+        <v>115</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>136</v>
+        <v>107</v>
       </c>
       <c r="B117">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="C117" t="s">
-        <v>66</v>
+        <v>116</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>180</v>
+        <v>107</v>
       </c>
       <c r="B118">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="C118" t="s">
-        <v>65</v>
+        <v>117</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>180</v>
+        <v>107</v>
       </c>
       <c r="B119">
-        <v>1</v>
+        <v>11</v>
       </c>
       <c r="C119" t="s">
-        <v>66</v>
+        <v>118</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B120">
         <v>0</v>
@@ -2294,7 +2309,7 @@
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B121">
         <v>1</v>
@@ -2305,7 +2320,7 @@
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B122">
         <v>0</v>
@@ -2316,7 +2331,7 @@
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>186</v>
+        <v>180</v>
       </c>
       <c r="B123">
         <v>1</v>
@@ -2327,7 +2342,7 @@
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>183</v>
+        <v>137</v>
       </c>
       <c r="B124">
         <v>0</v>
@@ -2338,7 +2353,7 @@
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>183</v>
+        <v>137</v>
       </c>
       <c r="B125">
         <v>1</v>
@@ -2349,7 +2364,7 @@
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B126">
         <v>0</v>
@@ -2360,7 +2375,7 @@
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="B127">
         <v>1</v>
@@ -2371,7 +2386,7 @@
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B128">
         <v>0</v>
@@ -2382,7 +2397,7 @@
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B129">
         <v>1</v>
@@ -2393,7 +2408,7 @@
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -2404,7 +2419,7 @@
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>190</v>
+        <v>184</v>
       </c>
       <c r="B131">
         <v>1</v>
@@ -2415,7 +2430,7 @@
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -2426,7 +2441,7 @@
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>202</v>
+        <v>185</v>
       </c>
       <c r="B133">
         <v>1</v>
@@ -2437,7 +2452,7 @@
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="B134">
         <v>0</v>
@@ -2448,7 +2463,7 @@
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
       <c r="B135">
         <v>1</v>
@@ -2459,7 +2474,7 @@
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B136">
         <v>0</v>
@@ -2470,7 +2485,7 @@
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B137">
         <v>1</v>
@@ -2481,7 +2496,7 @@
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="B138">
         <v>0</v>
@@ -2492,7 +2507,7 @@
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>192</v>
+        <v>204</v>
       </c>
       <c r="B139">
         <v>1</v>
@@ -2503,7 +2518,7 @@
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>144</v>
+        <v>203</v>
       </c>
       <c r="B140">
         <v>0</v>
@@ -2514,7 +2529,7 @@
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>144</v>
+        <v>203</v>
       </c>
       <c r="B141">
         <v>1</v>
@@ -2525,7 +2540,7 @@
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>155</v>
+        <v>192</v>
       </c>
       <c r="B142">
         <v>0</v>
@@ -2536,7 +2551,7 @@
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>155</v>
+        <v>192</v>
       </c>
       <c r="B143">
         <v>1</v>
@@ -2547,7 +2562,7 @@
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
       <c r="B144">
         <v>0</v>
@@ -2558,7 +2573,7 @@
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>176</v>
+        <v>144</v>
       </c>
       <c r="B145">
         <v>1</v>
@@ -2569,7 +2584,7 @@
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="B146">
         <v>0</v>
@@ -2580,7 +2595,7 @@
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="B147">
         <v>1</v>
@@ -2591,7 +2606,7 @@
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>142</v>
+        <v>176</v>
       </c>
       <c r="B148">
         <v>0</v>
@@ -2602,7 +2617,7 @@
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>142</v>
+        <v>176</v>
       </c>
       <c r="B149">
         <v>1</v>
@@ -2613,7 +2628,7 @@
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="B150">
         <v>0</v>
@@ -2624,7 +2639,7 @@
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>122</v>
+        <v>129</v>
       </c>
       <c r="B151">
         <v>1</v>
@@ -2635,7 +2650,7 @@
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="B152">
         <v>0</v>
@@ -2646,7 +2661,7 @@
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>154</v>
+        <v>142</v>
       </c>
       <c r="B153">
         <v>1</v>
@@ -2657,7 +2672,7 @@
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="B154">
         <v>0</v>
@@ -2668,7 +2683,7 @@
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>139</v>
+        <v>122</v>
       </c>
       <c r="B155">
         <v>1</v>
@@ -2679,7 +2694,7 @@
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="B156">
         <v>0</v>
@@ -2690,7 +2705,7 @@
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="B157">
         <v>1</v>
@@ -2701,7 +2716,7 @@
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B158">
         <v>0</v>
@@ -2712,7 +2727,7 @@
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="B159">
         <v>1</v>
@@ -2723,7 +2738,7 @@
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="B160">
         <v>0</v>
@@ -2734,7 +2749,7 @@
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>157</v>
+        <v>140</v>
       </c>
       <c r="B161">
         <v>1</v>
@@ -2745,7 +2760,7 @@
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="B162">
         <v>0</v>
@@ -2756,7 +2771,7 @@
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>173</v>
+        <v>138</v>
       </c>
       <c r="B163">
         <v>1</v>
@@ -2767,7 +2782,7 @@
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="B164">
         <v>0</v>
@@ -2778,7 +2793,7 @@
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>174</v>
+        <v>157</v>
       </c>
       <c r="B165">
         <v>1</v>
@@ -2789,7 +2804,7 @@
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B166">
         <v>0</v>
@@ -2800,7 +2815,7 @@
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B167">
         <v>1</v>
@@ -2811,7 +2826,7 @@
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>200</v>
+        <v>174</v>
       </c>
       <c r="B168">
         <v>0</v>
@@ -2822,7 +2837,7 @@
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>200</v>
+        <v>174</v>
       </c>
       <c r="B169">
         <v>1</v>
@@ -2833,7 +2848,7 @@
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="B170">
         <v>0</v>
@@ -2844,7 +2859,7 @@
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>198</v>
+        <v>178</v>
       </c>
       <c r="B171">
         <v>1</v>
@@ -2855,7 +2870,7 @@
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B172">
         <v>0</v>
@@ -2866,7 +2881,7 @@
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="B173">
         <v>1</v>
@@ -2877,7 +2892,7 @@
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B174">
         <v>0</v>
@@ -2888,7 +2903,7 @@
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="B175">
         <v>1</v>
@@ -2899,7 +2914,7 @@
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>134</v>
+        <v>199</v>
       </c>
       <c r="B176">
         <v>0</v>
@@ -2910,7 +2925,7 @@
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>134</v>
+        <v>199</v>
       </c>
       <c r="B177">
         <v>1</v>
@@ -2921,7 +2936,7 @@
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>126</v>
+        <v>201</v>
       </c>
       <c r="B178">
         <v>0</v>
@@ -2932,7 +2947,7 @@
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>126</v>
+        <v>201</v>
       </c>
       <c r="B179">
         <v>1</v>
@@ -2943,7 +2958,7 @@
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="B180">
         <v>0</v>
@@ -2954,7 +2969,7 @@
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>120</v>
+        <v>134</v>
       </c>
       <c r="B181">
         <v>1</v>
@@ -2965,7 +2980,7 @@
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="B182">
         <v>0</v>
@@ -2976,7 +2991,7 @@
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>145</v>
+        <v>126</v>
       </c>
       <c r="B183">
         <v>1</v>
@@ -2987,7 +3002,7 @@
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B184">
         <v>0</v>
@@ -2998,7 +3013,7 @@
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B185">
         <v>1</v>
@@ -3009,7 +3024,7 @@
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>187</v>
+        <v>145</v>
       </c>
       <c r="B186">
         <v>0</v>
@@ -3020,7 +3035,7 @@
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>187</v>
+        <v>145</v>
       </c>
       <c r="B187">
         <v>1</v>
@@ -3031,7 +3046,7 @@
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>167</v>
+        <v>123</v>
       </c>
       <c r="B188">
         <v>0</v>
@@ -3042,7 +3057,7 @@
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>167</v>
+        <v>123</v>
       </c>
       <c r="B189">
         <v>1</v>
@@ -3053,7 +3068,7 @@
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>158</v>
+        <v>187</v>
       </c>
       <c r="B190">
         <v>0</v>
@@ -3064,7 +3079,7 @@
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>158</v>
+        <v>187</v>
       </c>
       <c r="B191">
         <v>1</v>
@@ -3075,7 +3090,7 @@
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>130</v>
+        <v>167</v>
       </c>
       <c r="B192">
         <v>0</v>
@@ -3086,7 +3101,7 @@
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>130</v>
+        <v>167</v>
       </c>
       <c r="B193">
         <v>1</v>
@@ -3097,7 +3112,7 @@
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="B194">
         <v>0</v>
@@ -3108,7 +3123,7 @@
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>182</v>
+        <v>158</v>
       </c>
       <c r="B195">
         <v>1</v>
@@ -3119,7 +3134,7 @@
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>193</v>
+        <v>130</v>
       </c>
       <c r="B196">
         <v>0</v>
@@ -3130,7 +3145,7 @@
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>193</v>
+        <v>130</v>
       </c>
       <c r="B197">
         <v>1</v>
@@ -3141,7 +3156,7 @@
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>128</v>
+        <v>182</v>
       </c>
       <c r="B198">
         <v>0</v>
@@ -3152,7 +3167,7 @@
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>128</v>
+        <v>182</v>
       </c>
       <c r="B199">
         <v>1</v>
@@ -3163,7 +3178,7 @@
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="B200">
         <v>0</v>
@@ -3174,7 +3189,7 @@
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>171</v>
+        <v>193</v>
       </c>
       <c r="B201">
         <v>1</v>
@@ -3185,7 +3200,7 @@
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B202">
         <v>0</v>
@@ -3196,7 +3211,7 @@
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B203">
         <v>1</v>
@@ -3207,7 +3222,7 @@
     </row>
     <row r="204" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B204">
         <v>0</v>
@@ -3218,7 +3233,7 @@
     </row>
     <row r="205" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
-        <v>177</v>
+        <v>171</v>
       </c>
       <c r="B205">
         <v>1</v>
@@ -3229,7 +3244,7 @@
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="B206">
         <v>0</v>
@@ -3240,7 +3255,7 @@
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
-        <v>149</v>
+        <v>131</v>
       </c>
       <c r="B207">
         <v>1</v>
@@ -3251,7 +3266,7 @@
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B208">
         <v>0</v>
@@ -3262,7 +3277,7 @@
     </row>
     <row r="209" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B209">
         <v>1</v>
@@ -3273,7 +3288,7 @@
     </row>
     <row r="210" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="B210">
         <v>0</v>
@@ -3284,7 +3299,7 @@
     </row>
     <row r="211" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
-        <v>166</v>
+        <v>149</v>
       </c>
       <c r="B211">
         <v>1</v>
@@ -3295,7 +3310,7 @@
     </row>
     <row r="212" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="B212">
         <v>0</v>
@@ -3306,7 +3321,7 @@
     </row>
     <row r="213" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="B213">
         <v>1</v>
@@ -3317,7 +3332,7 @@
     </row>
     <row r="214" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
-        <v>119</v>
+        <v>166</v>
       </c>
       <c r="B214">
         <v>0</v>
@@ -3328,7 +3343,7 @@
     </row>
     <row r="215" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
-        <v>119</v>
+        <v>166</v>
       </c>
       <c r="B215">
         <v>1</v>
@@ -3339,7 +3354,7 @@
     </row>
     <row r="216" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="B216">
         <v>0</v>
@@ -3350,7 +3365,7 @@
     </row>
     <row r="217" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
-        <v>146</v>
+        <v>194</v>
       </c>
       <c r="B217">
         <v>1</v>
@@ -3361,7 +3376,7 @@
     </row>
     <row r="218" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
-        <v>195</v>
+        <v>119</v>
       </c>
       <c r="B218">
         <v>0</v>
@@ -3372,7 +3387,7 @@
     </row>
     <row r="219" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
-        <v>195</v>
+        <v>119</v>
       </c>
       <c r="B219">
         <v>1</v>
@@ -3383,7 +3398,7 @@
     </row>
     <row r="220" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="B220">
         <v>0</v>
@@ -3394,7 +3409,7 @@
     </row>
     <row r="221" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
-        <v>165</v>
+        <v>146</v>
       </c>
       <c r="B221">
         <v>1</v>
@@ -3405,7 +3420,7 @@
     </row>
     <row r="222" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
-        <v>170</v>
+        <v>195</v>
       </c>
       <c r="B222">
         <v>0</v>
@@ -3416,7 +3431,7 @@
     </row>
     <row r="223" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
-        <v>170</v>
+        <v>195</v>
       </c>
       <c r="B223">
         <v>1</v>
@@ -3427,7 +3442,7 @@
     </row>
     <row r="224" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
       <c r="B224">
         <v>0</v>
@@ -3438,7 +3453,7 @@
     </row>
     <row r="225" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
-        <v>127</v>
+        <v>165</v>
       </c>
       <c r="B225">
         <v>1</v>
@@ -3449,7 +3464,7 @@
     </row>
     <row r="226" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="B226">
         <v>0</v>
@@ -3460,7 +3475,7 @@
     </row>
     <row r="227" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
-        <v>147</v>
+        <v>170</v>
       </c>
       <c r="B227">
         <v>1</v>
@@ -3471,7 +3486,7 @@
     </row>
     <row r="228" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
-        <v>179</v>
+        <v>127</v>
       </c>
       <c r="B228">
         <v>0</v>
@@ -3482,7 +3497,7 @@
     </row>
     <row r="229" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
-        <v>179</v>
+        <v>127</v>
       </c>
       <c r="B229">
         <v>1</v>
@@ -3493,7 +3508,7 @@
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="B230">
         <v>0</v>
@@ -3504,7 +3519,7 @@
     </row>
     <row r="231" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
-        <v>133</v>
+        <v>147</v>
       </c>
       <c r="B231">
         <v>1</v>
@@ -3515,7 +3530,7 @@
     </row>
     <row r="232" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
-        <v>141</v>
+        <v>179</v>
       </c>
       <c r="B232">
         <v>0</v>
@@ -3526,7 +3541,7 @@
     </row>
     <row r="233" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
-        <v>141</v>
+        <v>179</v>
       </c>
       <c r="B233">
         <v>1</v>
@@ -3537,7 +3552,7 @@
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
-        <v>197</v>
+        <v>133</v>
       </c>
       <c r="B234">
         <v>0</v>
@@ -3548,7 +3563,7 @@
     </row>
     <row r="235" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
-        <v>197</v>
+        <v>133</v>
       </c>
       <c r="B235">
         <v>1</v>
@@ -3559,7 +3574,7 @@
     </row>
     <row r="236" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B236">
         <v>0</v>
@@ -3570,7 +3585,7 @@
     </row>
     <row r="237" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
-        <v>135</v>
+        <v>141</v>
       </c>
       <c r="B237">
         <v>1</v>
@@ -3581,7 +3596,7 @@
     </row>
     <row r="238" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B238">
         <v>0</v>
@@ -3592,7 +3607,7 @@
     </row>
     <row r="239" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="B239">
         <v>1</v>
@@ -3603,7 +3618,7 @@
     </row>
     <row r="240" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B240">
         <v>0</v>
@@ -3614,7 +3629,7 @@
     </row>
     <row r="241" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="B241">
         <v>1</v>
@@ -3625,7 +3640,7 @@
     </row>
     <row r="242" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
-        <v>125</v>
+        <v>189</v>
       </c>
       <c r="B242">
         <v>0</v>
@@ -3636,7 +3651,7 @@
     </row>
     <row r="243" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
-        <v>125</v>
+        <v>189</v>
       </c>
       <c r="B243">
         <v>1</v>
@@ -3647,7 +3662,7 @@
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="B244">
         <v>0</v>
@@ -3658,7 +3673,7 @@
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
-        <v>121</v>
+        <v>132</v>
       </c>
       <c r="B245">
         <v>1</v>
@@ -3669,7 +3684,7 @@
     </row>
     <row r="246" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
-        <v>196</v>
+        <v>125</v>
       </c>
       <c r="B246">
         <v>0</v>
@@ -3680,7 +3695,7 @@
     </row>
     <row r="247" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
-        <v>196</v>
+        <v>125</v>
       </c>
       <c r="B247">
         <v>1</v>
@@ -3691,7 +3706,7 @@
     </row>
     <row r="248" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
-        <v>148</v>
+        <v>121</v>
       </c>
       <c r="B248">
         <v>0</v>
@@ -3702,7 +3717,7 @@
     </row>
     <row r="249" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
-        <v>148</v>
+        <v>121</v>
       </c>
       <c r="B249">
         <v>1</v>
@@ -3713,7 +3728,7 @@
     </row>
     <row r="250" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B250">
         <v>0</v>
@@ -3724,7 +3739,7 @@
     </row>
     <row r="251" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
-        <v>188</v>
+        <v>196</v>
       </c>
       <c r="B251">
         <v>1</v>
@@ -3735,7 +3750,7 @@
     </row>
     <row r="252" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B252">
         <v>0</v>
@@ -3746,7 +3761,7 @@
     </row>
     <row r="253" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="B253">
         <v>1</v>
@@ -3757,7 +3772,7 @@
     </row>
     <row r="254" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
-        <v>41</v>
+        <v>188</v>
       </c>
       <c r="B254">
         <v>0</v>
@@ -3768,7 +3783,7 @@
     </row>
     <row r="255" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
-        <v>41</v>
+        <v>188</v>
       </c>
       <c r="B255">
         <v>1</v>
@@ -3779,7 +3794,7 @@
     </row>
     <row r="256" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="B256">
         <v>0</v>
@@ -3790,7 +3805,7 @@
     </row>
     <row r="257" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
-        <v>164</v>
+        <v>152</v>
       </c>
       <c r="B257">
         <v>1</v>
@@ -3801,7 +3816,7 @@
     </row>
     <row r="258" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
-        <v>163</v>
+        <v>41</v>
       </c>
       <c r="B258">
         <v>0</v>
@@ -3812,7 +3827,7 @@
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>163</v>
+        <v>41</v>
       </c>
       <c r="B259">
         <v>1</v>
@@ -3823,7 +3838,7 @@
     </row>
     <row r="260" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
-        <v>205</v>
+        <v>164</v>
       </c>
       <c r="B260">
         <v>0</v>
@@ -3834,7 +3849,7 @@
     </row>
     <row r="261" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
-        <v>205</v>
+        <v>164</v>
       </c>
       <c r="B261">
         <v>1</v>
@@ -3845,7 +3860,7 @@
     </row>
     <row r="262" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B262">
         <v>0</v>
@@ -3856,7 +3871,7 @@
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B263">
         <v>1</v>
@@ -3867,7 +3882,7 @@
     </row>
     <row r="264" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="B264">
         <v>0</v>
@@ -3878,7 +3893,7 @@
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
-        <v>191</v>
+        <v>205</v>
       </c>
       <c r="B265">
         <v>1</v>
@@ -3889,7 +3904,7 @@
     </row>
     <row r="266" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B266">
         <v>0</v>
@@ -3900,7 +3915,7 @@
     </row>
     <row r="267" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
-        <v>175</v>
+        <v>162</v>
       </c>
       <c r="B267">
         <v>1</v>
@@ -3911,7 +3926,7 @@
     </row>
     <row r="268" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
-        <v>153</v>
+        <v>191</v>
       </c>
       <c r="B268">
         <v>0</v>
@@ -3922,7 +3937,7 @@
     </row>
     <row r="269" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
-        <v>153</v>
+        <v>191</v>
       </c>
       <c r="B269">
         <v>1</v>
@@ -3933,7 +3948,7 @@
     </row>
     <row r="270" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
-        <v>143</v>
+        <v>175</v>
       </c>
       <c r="B270">
         <v>0</v>
@@ -3944,7 +3959,7 @@
     </row>
     <row r="271" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
-        <v>143</v>
+        <v>175</v>
       </c>
       <c r="B271">
         <v>1</v>
@@ -3955,7 +3970,7 @@
     </row>
     <row r="272" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B272">
         <v>0</v>
@@ -3966,7 +3981,7 @@
     </row>
     <row r="273" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="B273">
         <v>1</v>
@@ -3977,7 +3992,7 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
-        <v>172</v>
+        <v>143</v>
       </c>
       <c r="B274">
         <v>0</v>
@@ -3988,7 +4003,7 @@
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
-        <v>172</v>
+        <v>143</v>
       </c>
       <c r="B275">
         <v>1</v>
@@ -3999,7 +4014,7 @@
     </row>
     <row r="276" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B276">
         <v>0</v>
@@ -4010,7 +4025,7 @@
     </row>
     <row r="277" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="B277">
         <v>1</v>
@@ -4021,7 +4036,7 @@
     </row>
     <row r="278" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="B278">
         <v>0</v>
@@ -4032,7 +4047,7 @@
     </row>
     <row r="279" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
-        <v>159</v>
+        <v>172</v>
       </c>
       <c r="B279">
         <v>1</v>
@@ -4043,7 +4058,7 @@
     </row>
     <row r="280" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B280">
         <v>0</v>
@@ -4054,7 +4069,7 @@
     </row>
     <row r="281" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B281">
         <v>1</v>
@@ -4065,7 +4080,7 @@
     </row>
     <row r="282" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="B282">
         <v>0</v>
@@ -4076,7 +4091,7 @@
     </row>
     <row r="283" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
       <c r="B283">
         <v>1</v>
@@ -4087,7 +4102,7 @@
     </row>
     <row r="284" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="B284">
         <v>0</v>
@@ -4098,7 +4113,7 @@
     </row>
     <row r="285" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
-        <v>151</v>
+        <v>169</v>
       </c>
       <c r="B285">
         <v>1</v>
@@ -4109,7 +4124,7 @@
     </row>
     <row r="286" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="B286">
         <v>0</v>
@@ -4120,7 +4135,7 @@
     </row>
     <row r="287" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
-        <v>124</v>
+        <v>150</v>
       </c>
       <c r="B287">
         <v>1</v>
@@ -4131,7 +4146,7 @@
     </row>
     <row r="288" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B288">
         <v>0</v>
@@ -4142,7 +4157,7 @@
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B289">
         <v>1</v>
@@ -4153,7 +4168,7 @@
     </row>
     <row r="290" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
-        <v>161</v>
+        <v>124</v>
       </c>
       <c r="B290">
         <v>0</v>
@@ -4164,12 +4179,56 @@
     </row>
     <row r="291" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
+        <v>124</v>
+      </c>
+      <c r="B291">
+        <v>1</v>
+      </c>
+      <c r="C291" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="292" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>160</v>
+      </c>
+      <c r="B292">
+        <v>0</v>
+      </c>
+      <c r="C292" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="293" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A293" t="s">
+        <v>160</v>
+      </c>
+      <c r="B293">
+        <v>1</v>
+      </c>
+      <c r="C293" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="294" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A294" t="s">
         <v>161</v>
       </c>
-      <c r="B291">
-        <v>1</v>
-      </c>
-      <c r="C291" t="s">
+      <c r="B294">
+        <v>0</v>
+      </c>
+      <c r="C294" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="295" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>161</v>
+      </c>
+      <c r="B295">
+        <v>1</v>
+      </c>
+      <c r="C295" t="s">
         <v>66</v>
       </c>
     </row>

</xml_diff>